<commit_message>
Python Week 2 Day 3
</commit_message>
<xml_diff>
--- a/python_excel/data9.xlsx
+++ b/python_excel/data9.xlsx
@@ -1,33 +1,79 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Trainees" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>Data 9</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Andy</t>
+  </si>
+  <si>
+    <t>Ben</t>
+  </si>
+  <si>
+    <t>CJ</t>
+  </si>
+  <si>
+    <t>Gigi</t>
+  </si>
+  <si>
+    <t>Johnny</t>
+  </si>
+  <si>
+    <t>Khanhi</t>
+  </si>
+  <si>
+    <t>Sassy</t>
+  </si>
+  <si>
+    <t>Shugs</t>
+  </si>
+  <si>
+    <t>Tosin</t>
+  </si>
+  <si>
+    <t>Vivek</t>
+  </si>
+  <si>
+    <t>Weiyee</t>
+  </si>
+  <si>
+    <t>Yin</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,11 +92,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -339,115 +386,81 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>changed</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>First Name</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Andy</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Ben</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>CJ</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Gigi</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Johnny</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Khanhi</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Sassy</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Shugs</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Tosin</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Vivek</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Weiyee</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Yin</t>
-        </is>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>